<commit_message>
Coreccion de errores InterAlliance e InterChange
</commit_message>
<xml_diff>
--- a/DOCUMENTOS/Libro1_pruebas.xlsx
+++ b/DOCUMENTOS/Libro1_pruebas.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2039" uniqueCount="1417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="1435">
   <si>
     <t>ID</t>
   </si>
@@ -4277,6 +4278,60 @@
   </si>
   <si>
     <t>Vaticano</t>
+  </si>
+  <si>
+    <t>INICIATIVA</t>
+  </si>
+  <si>
+    <t>INSCRIPCION</t>
+  </si>
+  <si>
+    <t>INSTITUCION</t>
+  </si>
+  <si>
+    <t>OPORTUNIDAD</t>
+  </si>
+  <si>
+    <t>MULTIMEDIA</t>
+  </si>
+  <si>
+    <t>ALIANZA</t>
+  </si>
+  <si>
+    <t>IDENTIDAD</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>EMAIL -</t>
+  </si>
+  <si>
+    <t>REGISTRO DATOS EL USUARIO</t>
+  </si>
+  <si>
+    <t>RECHAZADO POR EL VALIDADOR</t>
+  </si>
+  <si>
+    <t>APROBADO POR EL VALIDADOR</t>
+  </si>
+  <si>
+    <t>ACTIVA POR EL VALIDADOR</t>
+  </si>
+  <si>
+    <t>VENCIDA PARA INVOLUCRADOS</t>
+  </si>
+  <si>
+    <t>ACTIVA PARA INVOLUCRADOS</t>
+  </si>
+  <si>
+    <t>REGISTRO DATOS EL USUARIO EXTERNO</t>
+  </si>
+  <si>
+    <t>ACEPTADO POR EL USUARIO EXTERNO</t>
+  </si>
+  <si>
+    <t>DECLINADO POR EL USUARIO EXTERNO</t>
   </si>
 </sst>
 </file>
@@ -4314,12 +4369,14 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4484,7 +4541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -4590,6 +4647,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -5907,7 +5965,7 @@
   <dimension ref="B2:AO113"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6065,24 +6123,24 @@
       </c>
       <c r="N9" s="11" t="str">
         <f t="shared" ref="N9:N40" ca="1" si="0">INDEX(I$9:I$16,RANDBETWEEN(1,COUNTA(I$9:I$16)))</f>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O9" s="11" t="str">
         <f t="shared" ref="O9:O40" ca="1" si="1">INDEX(K$9:K$21,RANDBETWEEN(1,COUNTA(K$9:K$21)))</f>
-        <v>Doble Titulación</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="Q9" s="11" t="str">
         <f t="shared" ref="Q9:Q40" ca="1" si="2">INDEX(J$9:J$22,RANDBETWEEN(1,COUNTA(J$9:J$22)))</f>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R9" s="13"/>
       <c r="S9" s="11"/>
       <c r="T9" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Jennifer&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Jennifer&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U9" s="15"/>
       <c r="V9" s="15" t="s">
@@ -6137,24 +6195,24 @@
       </c>
       <c r="N10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O10" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q10" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R10" s="13"/>
       <c r="S10" s="11"/>
       <c r="T10" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Clark&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Clark&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U10" s="15"/>
       <c r="V10" s="15" t="s">
@@ -6209,24 +6267,24 @@
       </c>
       <c r="N11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O11" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Prácticas</v>
+        <v>Voluntariado Impacta Brasil</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="Q11" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R11" s="13"/>
       <c r="S11" s="11"/>
       <c r="T11" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Brendan&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Brendan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U11" s="15"/>
       <c r="V11" s="15" t="s">
@@ -6285,20 +6343,20 @@
       </c>
       <c r="O12" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="Q12" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="11"/>
       <c r="T12" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Warren&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Warren&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U12" s="15"/>
       <c r="V12" s="15" t="s">
@@ -6353,24 +6411,24 @@
       </c>
       <c r="N13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O13" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Summer Programme Responsible Management Rennes</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="Q13" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R13" s="13"/>
       <c r="S13" s="11"/>
       <c r="T13" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Rajah&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Rajah&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15" t="s">
@@ -6425,24 +6483,24 @@
       </c>
       <c r="N14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O14" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q14" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R14" s="13"/>
       <c r="S14" s="11"/>
       <c r="T14" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Demetrius&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Demetrius&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U14" s="15"/>
       <c r="V14" s="15" t="s">
@@ -6460,7 +6518,7 @@
       <c r="Z14" s="21"/>
       <c r="AA14" s="21"/>
     </row>
-    <row r="15" spans="2:27" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:27" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
@@ -6497,24 +6555,24 @@
       </c>
       <c r="N15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O15" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="Q15" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="11"/>
       <c r="T15" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Keefe&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Keefe&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U15" s="15"/>
       <c r="V15" s="15" t="s">
@@ -6569,24 +6627,24 @@
       </c>
       <c r="N16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O16" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>40</v>
       </c>
       <c r="Q16" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R16" s="13"/>
       <c r="S16" s="11"/>
       <c r="T16" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Leila&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Leila&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U16" s="15"/>
       <c r="V16" s="15" t="s">
@@ -6639,24 +6697,24 @@
       </c>
       <c r="N17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O17" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Korean Studies Summer Program Hannam University</v>
+        <v>Prácticas</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="Q17" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R17" s="13"/>
       <c r="S17" s="11"/>
       <c r="T17" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Fritz&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Fritz&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U17" s="15"/>
       <c r="V17" s="15" t="s">
@@ -6709,24 +6767,24 @@
       </c>
       <c r="N18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O18" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Semestre Académico</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>49</v>
       </c>
       <c r="Q18" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R18" s="13"/>
       <c r="S18" s="11"/>
       <c r="T18" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Cassady&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Cassady&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U18" s="15"/>
       <c r="V18" s="15" t="s">
@@ -6783,20 +6841,20 @@
       </c>
       <c r="O19" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta México</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="Q19" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R19" s="13"/>
       <c r="S19" s="11"/>
       <c r="T19" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Rogan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Rogan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U19" s="15"/>
       <c r="V19" s="15" t="s">
@@ -6849,24 +6907,24 @@
       </c>
       <c r="N20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O20" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Prácticas</v>
+        <v>Voluntariado impacta Perú</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>59</v>
       </c>
       <c r="Q20" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R20" s="13"/>
       <c r="S20" s="11"/>
       <c r="T20" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Candice&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Candice&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U20" s="15"/>
       <c r="V20" s="15" t="s">
@@ -6919,24 +6977,24 @@
       </c>
       <c r="N21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O21" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gira Académica Italia</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>64</v>
       </c>
       <c r="Q21" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R21" s="13"/>
       <c r="S21" s="11"/>
       <c r="T21" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Brittany&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Brittany&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U21" s="15"/>
       <c r="V21" s="15" t="s">
@@ -6990,24 +7048,24 @@
       </c>
       <c r="N22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O22" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>69</v>
       </c>
       <c r="Q22" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R22" s="13"/>
       <c r="S22" s="11"/>
       <c r="T22" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Baxter&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Baxter&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U22" s="15"/>
       <c r="V22" s="15" t="s">
@@ -7059,7 +7117,7 @@
       </c>
       <c r="N23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>JUNIO A JULIO 2018</v>
       </c>
       <c r="O23" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7070,13 +7128,13 @@
       </c>
       <c r="Q23" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R23" s="13"/>
       <c r="S23" s="11"/>
       <c r="T23" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Vaughan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Vaughan&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U23" s="15"/>
       <c r="V23" s="15" t="s">
@@ -7125,24 +7183,24 @@
       </c>
       <c r="N24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>JUNIO A JULIO 2018</v>
       </c>
       <c r="O24" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Summer Programme Responsible Management Rennes</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>80</v>
       </c>
       <c r="Q24" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R24" s="13"/>
       <c r="S24" s="11"/>
       <c r="T24" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Ivan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Ivan&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U24" s="15"/>
       <c r="V24" s="15"/>
@@ -7183,24 +7241,24 @@
       </c>
       <c r="N25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O25" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P25" s="3" t="s">
         <v>85</v>
       </c>
       <c r="Q25" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R25" s="13"/>
       <c r="S25" s="11"/>
       <c r="T25" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Marah&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Marah&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
@@ -7210,7 +7268,7 @@
       <c r="Z25" s="21"/>
       <c r="AA25" s="21"/>
     </row>
-    <row r="26" spans="2:41" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:41" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>18</v>
       </c>
@@ -7241,24 +7299,24 @@
       </c>
       <c r="N26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O26" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Doble Titulación</v>
+        <v>Voluntariado impacta México</v>
       </c>
       <c r="P26" s="5" t="s">
         <v>90</v>
       </c>
       <c r="Q26" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R26" s="13"/>
       <c r="S26" s="11"/>
       <c r="T26" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Kiara&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Kiara&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
@@ -7299,24 +7357,24 @@
       </c>
       <c r="N27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O27" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Gira Académica Italia</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P27" s="3" t="s">
         <v>95</v>
       </c>
       <c r="Q27" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R27" s="13"/>
       <c r="S27" s="11"/>
       <c r="T27" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Brielle&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Brielle&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U27" s="15"/>
       <c r="V27" s="15" t="s">
@@ -7365,24 +7423,24 @@
       </c>
       <c r="N28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O28" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Voluntariado Impacta Brasil</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>100</v>
       </c>
       <c r="Q28" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R28" s="13"/>
       <c r="S28" s="11"/>
       <c r="T28" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Kennedy&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Kennedy&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U28" s="15"/>
       <c r="V28" s="15" t="s">
@@ -7431,7 +7489,7 @@
       </c>
       <c r="N29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O29" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7442,13 +7500,13 @@
       </c>
       <c r="Q29" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R29" s="13"/>
       <c r="S29" s="11"/>
       <c r="T29" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Peter&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Peter&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U29" s="15"/>
       <c r="V29" s="15" t="s">
@@ -7497,24 +7555,24 @@
       </c>
       <c r="N30" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O30" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P30" s="5" t="s">
         <v>110</v>
       </c>
       <c r="Q30" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R30" s="13"/>
       <c r="S30" s="11"/>
       <c r="T30" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Kibo&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Kibo&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U30" s="15"/>
       <c r="V30" s="15"/>
@@ -7555,7 +7613,7 @@
       </c>
       <c r="N31" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O31" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7566,13 +7624,13 @@
       </c>
       <c r="Q31" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
       </c>
       <c r="R31" s="13"/>
       <c r="S31" s="11"/>
       <c r="T31" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Tanek&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Tanek&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U31" s="15"/>
       <c r="V31" s="15" t="s">
@@ -7625,20 +7683,20 @@
       </c>
       <c r="O32" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Semestre Académico</v>
+        <v>Voluntariado impacta México</v>
       </c>
       <c r="P32" s="5" t="s">
         <v>119</v>
       </c>
       <c r="Q32" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R32" s="13"/>
       <c r="S32" s="11"/>
       <c r="T32" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Guinevere&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Guinevere&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U32" s="15"/>
       <c r="V32" s="15" t="s">
@@ -7687,11 +7745,11 @@
       </c>
       <c r="N33" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O33" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Voluntariado impacta Perú</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>124</v>
@@ -7704,7 +7762,7 @@
       <c r="S33" s="11"/>
       <c r="T33" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Ronan&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Ronan&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U33" s="15"/>
       <c r="V33" s="15" t="s">
@@ -7753,24 +7811,24 @@
       </c>
       <c r="N34" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O34" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Prácticas</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>128</v>
       </c>
       <c r="Q34" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R34" s="13"/>
       <c r="S34" s="11"/>
       <c r="T34" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Kasper&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Kasper&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U34" s="15"/>
       <c r="V34" s="15" t="s">
@@ -7819,24 +7877,24 @@
       </c>
       <c r="N35" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O35" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P35" s="3" t="s">
         <v>133</v>
       </c>
       <c r="Q35" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R35" s="13"/>
       <c r="S35" s="11"/>
       <c r="T35" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Otto&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Otto&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U35" s="15"/>
       <c r="V35" s="15" t="s">
@@ -7885,24 +7943,24 @@
       </c>
       <c r="N36" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O36" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta México</v>
+        <v>Korean Studies Summer Program Hannam University</v>
       </c>
       <c r="P36" s="5" t="s">
         <v>139</v>
       </c>
       <c r="Q36" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R36" s="13"/>
       <c r="S36" s="11"/>
       <c r="T36" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Brenda&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Brenda&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U36" s="15"/>
       <c r="V36" s="15" t="s">
@@ -7951,7 +8009,7 @@
       </c>
       <c r="N37" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O37" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7962,13 +8020,13 @@
       </c>
       <c r="Q37" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R37" s="13"/>
       <c r="S37" s="11"/>
       <c r="T37" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Laith&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Laith&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U37" s="15"/>
       <c r="V37" s="15" t="s">
@@ -8017,24 +8075,24 @@
       </c>
       <c r="N38" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O38" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado Impacta Brasil</v>
+        <v>Voluntariado impacta México</v>
       </c>
       <c r="P38" s="5" t="s">
         <v>149</v>
       </c>
       <c r="Q38" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R38" s="13"/>
       <c r="S38" s="11"/>
       <c r="T38" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Ella&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Ella&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U38" s="15"/>
       <c r="V38" s="15"/>
@@ -8075,7 +8133,7 @@
       </c>
       <c r="N39" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O39" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -8086,13 +8144,13 @@
       </c>
       <c r="Q39" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R39" s="13"/>
       <c r="S39" s="11"/>
       <c r="T39" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Hanae&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Hanae&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U39" s="15"/>
       <c r="V39" s="15" t="s">
@@ -8141,24 +8199,24 @@
       </c>
       <c r="N40" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O40" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P40" s="5" t="s">
         <v>160</v>
       </c>
       <c r="Q40" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R40" s="13"/>
       <c r="S40" s="11"/>
       <c r="T40" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Donna&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Donna&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U40" s="15"/>
       <c r="V40" s="15" t="s">
@@ -8207,11 +8265,11 @@
       </c>
       <c r="N41" s="11" t="str">
         <f t="shared" ref="N41:N72" ca="1" si="3">INDEX(I$9:I$16,RANDBETWEEN(1,COUNTA(I$9:I$16)))</f>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O41" s="11" t="str">
         <f t="shared" ref="O41:O72" ca="1" si="4">INDEX(K$9:K$21,RANDBETWEEN(1,COUNTA(K$9:K$21)))</f>
-        <v>Voluntariado impacta Perú</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P41" s="3" t="s">
         <v>165</v>
@@ -8224,7 +8282,7 @@
       <c r="S41" s="11"/>
       <c r="T41" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Bevis&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Bevis&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U41" s="15"/>
       <c r="V41" s="15" t="s">
@@ -8273,24 +8331,24 @@
       </c>
       <c r="N42" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O42" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Doble Titulación</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P42" s="5" t="s">
         <v>170</v>
       </c>
       <c r="Q42" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R42" s="13"/>
       <c r="S42" s="11"/>
       <c r="T42" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Celeste&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Celeste&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U42" s="15"/>
       <c r="V42" s="15" t="s">
@@ -8339,24 +8397,24 @@
       </c>
       <c r="N43" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O43" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Korean Studies Summer Program Hannam University</v>
       </c>
       <c r="P43" s="3" t="s">
         <v>175</v>
       </c>
       <c r="Q43" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R43" s="13"/>
       <c r="S43" s="11"/>
       <c r="T43" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Ila&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Ila&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U43" s="15"/>
       <c r="V43" s="15" t="s">
@@ -8405,24 +8463,24 @@
       </c>
       <c r="N44" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O44" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>181</v>
       </c>
       <c r="Q44" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R44" s="13"/>
       <c r="S44" s="11"/>
       <c r="T44" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Alana&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Alana&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U44" s="15"/>
       <c r="V44" s="15" t="s">
@@ -8475,20 +8533,20 @@
       </c>
       <c r="O45" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Doble Titulación</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P45" s="3" t="s">
         <v>185</v>
       </c>
       <c r="Q45" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R45" s="13"/>
       <c r="S45" s="11"/>
       <c r="T45" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Rowan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Rowan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U45" s="15"/>
       <c r="V45" s="15" t="s">
@@ -8537,24 +8595,24 @@
       </c>
       <c r="N46" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O46" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Doble Titulación</v>
+        <v>Voluntariado impacta Perú</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>189</v>
       </c>
       <c r="Q46" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R46" s="13"/>
       <c r="S46" s="11"/>
       <c r="T46" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Eric&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Eric&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U46" s="15"/>
       <c r="V46" s="15" t="s">
@@ -8603,24 +8661,24 @@
       </c>
       <c r="N47" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O47" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P47" s="3" t="s">
         <v>194</v>
       </c>
       <c r="Q47" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R47" s="13"/>
       <c r="S47" s="11"/>
       <c r="T47" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Dana&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Dana&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U47" s="15"/>
       <c r="V47" s="15" t="s">
@@ -8669,24 +8727,24 @@
       </c>
       <c r="N48" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O48" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Korean Studies Summer Program Hannam University</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P48" s="5" t="s">
         <v>200</v>
       </c>
       <c r="Q48" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R48" s="13"/>
       <c r="S48" s="11"/>
       <c r="T48" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Karleigh&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Karleigh&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U48" s="15"/>
       <c r="V48" s="15" t="s">
@@ -8739,20 +8797,20 @@
       </c>
       <c r="O49" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Korean Studies Summer Program Hannam University</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>204</v>
       </c>
       <c r="Q49" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R49" s="13"/>
       <c r="S49" s="11"/>
       <c r="T49" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Malik&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Malik&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U49" s="15"/>
       <c r="V49" s="15" t="s">
@@ -8801,7 +8859,7 @@
       </c>
       <c r="N50" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O50" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -8812,13 +8870,13 @@
       </c>
       <c r="Q50" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
       </c>
       <c r="R50" s="13"/>
       <c r="S50" s="11"/>
       <c r="T50" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;May&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;May&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U50" s="15"/>
       <c r="V50" s="15" t="s">
@@ -8867,24 +8925,24 @@
       </c>
       <c r="N51" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O51" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>214</v>
       </c>
       <c r="Q51" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R51" s="13"/>
       <c r="S51" s="11"/>
       <c r="T51" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Alan&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Alan&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U51" s="15"/>
       <c r="V51" s="15"/>
@@ -8925,7 +8983,7 @@
       </c>
       <c r="N52" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O52" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -8936,13 +8994,13 @@
       </c>
       <c r="Q52" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R52" s="13"/>
       <c r="S52" s="11"/>
       <c r="T52" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Anastasia&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Anastasia&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U52" s="15"/>
       <c r="V52" s="15" t="s">
@@ -8991,24 +9049,24 @@
       </c>
       <c r="N53" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O53" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P53" s="3" t="s">
         <v>223</v>
       </c>
       <c r="Q53" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R53" s="13"/>
       <c r="S53" s="11"/>
       <c r="T53" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Yardley&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Yardley&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U53" s="15"/>
       <c r="V53" s="15" t="s">
@@ -9061,20 +9119,20 @@
       </c>
       <c r="O54" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P54" s="5" t="s">
         <v>228</v>
       </c>
       <c r="Q54" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R54" s="13"/>
       <c r="S54" s="11"/>
       <c r="T54" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Oscar&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Oscar&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U54" s="15"/>
       <c r="V54" s="15" t="s">
@@ -9123,24 +9181,24 @@
       </c>
       <c r="N55" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O55" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Voluntariado impacta México</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P55" s="3" t="s">
         <v>234</v>
       </c>
       <c r="Q55" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R55" s="13"/>
       <c r="S55" s="11"/>
       <c r="T55" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Hasad&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Hasad&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U55" s="15"/>
       <c r="V55" s="15" t="s">
@@ -9189,24 +9247,24 @@
       </c>
       <c r="N56" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O56" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Doble Titulación</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P56" s="5" t="s">
         <v>240</v>
       </c>
       <c r="Q56" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R56" s="13"/>
       <c r="S56" s="11"/>
       <c r="T56" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Mohammad&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/08/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Mohammad&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U56" s="15"/>
       <c r="V56" s="15" t="s">
@@ -9255,24 +9313,24 @@
       </c>
       <c r="N57" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O57" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Doble Titulación</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P57" s="3" t="s">
         <v>244</v>
       </c>
       <c r="Q57" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R57" s="13"/>
       <c r="S57" s="11"/>
       <c r="T57" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Nissim&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Nissim&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U57" s="15"/>
       <c r="V57" s="15" t="s">
@@ -9321,24 +9379,24 @@
       </c>
       <c r="N58" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O58" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Semestre Académico</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>250</v>
       </c>
       <c r="Q58" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R58" s="13"/>
       <c r="S58" s="11"/>
       <c r="T58" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Porter&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Porter&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U58" s="15"/>
       <c r="V58" s="15" t="s">
@@ -9387,24 +9445,24 @@
       </c>
       <c r="N59" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>JUNIO A JULIO 2018</v>
       </c>
       <c r="O59" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Gira Académica Italia</v>
+        <v>Summer Programme Responsible Management Rennes</v>
       </c>
       <c r="P59" s="3" t="s">
         <v>254</v>
       </c>
       <c r="Q59" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
       </c>
       <c r="R59" s="13"/>
       <c r="S59" s="11"/>
       <c r="T59" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Sophia&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Sophia&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U59" s="15"/>
       <c r="V59" s="15" t="s">
@@ -9453,24 +9511,24 @@
       </c>
       <c r="N60" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O60" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Prácticas</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>259</v>
       </c>
       <c r="Q60" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R60" s="13"/>
       <c r="S60" s="11"/>
       <c r="T60" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Acton&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Acton&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U60" s="15"/>
       <c r="V60" s="15" t="s">
@@ -9523,20 +9581,20 @@
       </c>
       <c r="O61" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>264</v>
       </c>
       <c r="Q61" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R61" s="13"/>
       <c r="S61" s="11"/>
       <c r="T61" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Briar&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Briar&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U61" s="15"/>
       <c r="V61" s="15" t="s">
@@ -9585,24 +9643,24 @@
       </c>
       <c r="N62" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O62" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Voluntariado impacta México</v>
+        <v>Voluntariado impacta Perú</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>268</v>
       </c>
       <c r="Q62" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R62" s="13"/>
       <c r="S62" s="11"/>
       <c r="T62" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Benjamin&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Benjamin&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U62" s="15"/>
       <c r="V62" s="15" t="s">
@@ -9651,24 +9709,24 @@
       </c>
       <c r="N63" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O63" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P63" s="3" t="s">
         <v>274</v>
       </c>
       <c r="Q63" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
       </c>
       <c r="R63" s="13"/>
       <c r="S63" s="11"/>
       <c r="T63" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Gregory&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Gregory&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U63" s="15"/>
       <c r="V63" s="15" t="s">
@@ -9717,24 +9775,24 @@
       </c>
       <c r="N64" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O64" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Gira Académica Italia</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>278</v>
       </c>
       <c r="Q64" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R64" s="13"/>
       <c r="S64" s="11"/>
       <c r="T64" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Marny&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Marny&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U64" s="15"/>
       <c r="V64" s="15"/>
@@ -9775,24 +9833,24 @@
       </c>
       <c r="N65" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O65" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v>Prácticas</v>
       </c>
       <c r="P65" s="3" t="s">
         <v>282</v>
       </c>
       <c r="Q65" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R65" s="13"/>
       <c r="S65" s="11"/>
       <c r="T65" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Indira&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Indira&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U65" s="15"/>
       <c r="V65" s="15"/>
@@ -9833,11 +9891,11 @@
       </c>
       <c r="N66" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O66" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>286</v>
@@ -9850,7 +9908,7 @@
       <c r="S66" s="11"/>
       <c r="T66" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Fleur&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/09/2012&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Fleur&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U66" s="15"/>
       <c r="V66" s="15" t="s">
@@ -9868,7 +9926,7 @@
       <c r="Z66" s="21"/>
       <c r="AA66" s="21"/>
     </row>
-    <row r="67" spans="2:27" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:27" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="3">
         <v>59</v>
       </c>
@@ -9899,24 +9957,24 @@
       </c>
       <c r="N67" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O67" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P67" s="3" t="s">
         <v>292</v>
       </c>
       <c r="Q67" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R67" s="13"/>
       <c r="S67" s="11"/>
       <c r="T67" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Fulton&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Fulton&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U67" s="15"/>
       <c r="V67" s="15" t="s">
@@ -9969,20 +10027,20 @@
       </c>
       <c r="O68" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>297</v>
       </c>
       <c r="Q68" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R68" s="13"/>
       <c r="S68" s="11"/>
       <c r="T68" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Arsenio&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Arsenio&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U68" s="15"/>
       <c r="V68" s="15" t="s">
@@ -10031,24 +10089,24 @@
       </c>
       <c r="N69" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O69" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P69" s="3" t="s">
         <v>302</v>
       </c>
       <c r="Q69" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R69" s="13"/>
       <c r="S69" s="11"/>
       <c r="T69" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Jaden&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Jaden&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U69" s="15"/>
       <c r="V69" s="15" t="s">
@@ -10097,24 +10155,24 @@
       </c>
       <c r="N70" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O70" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>307</v>
       </c>
       <c r="Q70" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R70" s="13"/>
       <c r="S70" s="11"/>
       <c r="T70" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Kylie&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;07/08/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Kylie&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U70" s="15"/>
       <c r="V70" s="15" t="s">
@@ -10167,20 +10225,20 @@
       </c>
       <c r="O71" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P71" s="3" t="s">
         <v>313</v>
       </c>
       <c r="Q71" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R71" s="13"/>
       <c r="S71" s="11"/>
       <c r="T71" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Melyssa&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/03/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Melyssa&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U71" s="15"/>
       <c r="V71" s="15" t="s">
@@ -10229,24 +10287,24 @@
       </c>
       <c r="N72" s="11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O72" s="11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Prácticas</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>318</v>
       </c>
       <c r="Q72" s="11" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R72" s="13"/>
       <c r="S72" s="11"/>
       <c r="T72" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Jerry&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Jerry&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U72" s="15"/>
       <c r="V72" s="15" t="s">
@@ -10299,20 +10357,20 @@
       </c>
       <c r="O73" s="11" t="str">
         <f t="shared" ref="O73:O108" ca="1" si="7">INDEX(K$9:K$21,RANDBETWEEN(1,COUNTA(K$9:K$21)))</f>
-        <v>Gira Académica Italia</v>
+        <v>Prácticas</v>
       </c>
       <c r="P73" s="3" t="s">
         <v>323</v>
       </c>
       <c r="Q73" s="11" t="str">
         <f t="shared" ref="Q73:Q108" ca="1" si="8">INDEX(J$9:J$22,RANDBETWEEN(1,COUNTA(J$9:J$22)))</f>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R73" s="13"/>
       <c r="S73" s="11"/>
       <c r="T73" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Rhiannon&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Rhiannon&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U73" s="15"/>
       <c r="V73" s="15" t="s">
@@ -10361,7 +10419,7 @@
       </c>
       <c r="N74" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O74" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -10372,13 +10430,13 @@
       </c>
       <c r="Q74" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R74" s="13"/>
       <c r="S74" s="11"/>
       <c r="T74" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Price&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;10/07/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Price&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U74" s="15"/>
       <c r="V74" s="15" t="s">
@@ -10427,24 +10485,24 @@
       </c>
       <c r="N75" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O75" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P75" s="3" t="s">
         <v>333</v>
       </c>
       <c r="Q75" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
       </c>
       <c r="R75" s="13"/>
       <c r="S75" s="11"/>
       <c r="T75" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Ginger&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Ginger&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U75" s="15"/>
       <c r="V75" s="15" t="s">
@@ -10497,20 +10555,20 @@
       </c>
       <c r="O76" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P76" s="5" t="s">
         <v>338</v>
       </c>
       <c r="Q76" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R76" s="13"/>
       <c r="S76" s="11"/>
       <c r="T76" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Britanney&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Britanney&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U76" s="15"/>
       <c r="V76" s="15" t="s">
@@ -10559,7 +10617,7 @@
       </c>
       <c r="N77" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O77" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -10570,13 +10628,13 @@
       </c>
       <c r="Q77" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R77" s="13"/>
       <c r="S77" s="11"/>
       <c r="T77" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Wylie&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Wylie&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U77" s="15"/>
       <c r="V77" s="15" t="s">
@@ -10625,7 +10683,7 @@
       </c>
       <c r="N78" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O78" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -10636,13 +10694,13 @@
       </c>
       <c r="Q78" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R78" s="13"/>
       <c r="S78" s="11"/>
       <c r="T78" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Holly&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Holly&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U78" s="15"/>
       <c r="V78" s="15" t="s">
@@ -10691,24 +10749,24 @@
       </c>
       <c r="N79" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SEGUNDO SEMESTRE 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O79" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Doble Titulación</v>
+        <v>Korean Studies Summer Program Hannam University</v>
       </c>
       <c r="P79" s="3" t="s">
         <v>353</v>
       </c>
       <c r="Q79" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R79" s="13"/>
       <c r="S79" s="11"/>
       <c r="T79" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Althea&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Althea&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U79" s="15"/>
       <c r="V79" s="15" t="s">
@@ -10757,24 +10815,24 @@
       </c>
       <c r="N80" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O80" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Korean Studies Summer Program Hannam University</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>358</v>
       </c>
       <c r="Q80" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R80" s="13"/>
       <c r="S80" s="11"/>
       <c r="T80" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Quintessa&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/06/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Quintessa&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U80" s="15"/>
       <c r="V80" s="15" t="s">
@@ -10823,24 +10881,24 @@
       </c>
       <c r="N81" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O81" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v xml:space="preserve">  Gira Académica a Perú</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P81" s="3" t="s">
         <v>361</v>
       </c>
       <c r="Q81" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R81" s="13"/>
       <c r="S81" s="11"/>
       <c r="T81" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Fitzgerald&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Fitzgerald&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U81" s="15"/>
       <c r="V81" s="15" t="s">
@@ -10858,7 +10916,7 @@
       <c r="Z81" s="21"/>
       <c r="AA81" s="21"/>
     </row>
-    <row r="82" spans="2:27" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:27" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="5">
         <v>74</v>
       </c>
@@ -10893,20 +10951,20 @@
       </c>
       <c r="O82" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Gira Académica Italia</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P82" s="5" t="s">
         <v>35</v>
       </c>
       <c r="Q82" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R82" s="13"/>
       <c r="S82" s="11"/>
       <c r="T82" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Keefe&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Keefe&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U82" s="15"/>
       <c r="V82" s="15" t="s">
@@ -10955,11 +11013,11 @@
       </c>
       <c r="N83" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O83" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P83" s="3" t="s">
         <v>370</v>
@@ -10972,7 +11030,7 @@
       <c r="S83" s="11"/>
       <c r="T83" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Rudyard&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Rudyard&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U83" s="15"/>
       <c r="V83" s="15" t="s">
@@ -11021,11 +11079,11 @@
       </c>
       <c r="N84" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O84" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Semestre Académico</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P84" s="5" t="s">
         <v>375</v>
@@ -11038,7 +11096,7 @@
       <c r="S84" s="11"/>
       <c r="T84" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Kareem&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/01/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Kareem&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U84" s="15"/>
       <c r="V84" s="15" t="s">
@@ -11087,24 +11145,24 @@
       </c>
       <c r="N85" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O85" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Korean Studies Summer Program Hannam University</v>
       </c>
       <c r="P85" s="3" t="s">
         <v>380</v>
       </c>
       <c r="Q85" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R85" s="13"/>
       <c r="S85" s="11"/>
       <c r="T85" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Genevieve&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Genevieve&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U85" s="15"/>
       <c r="V85" s="15" t="s">
@@ -11153,24 +11211,24 @@
       </c>
       <c r="N86" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O86" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Gira Académica Italia</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P86" s="5" t="s">
         <v>385</v>
       </c>
       <c r="Q86" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R86" s="13"/>
       <c r="S86" s="11"/>
       <c r="T86" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Wang&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;04/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Wang&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U86" s="15"/>
       <c r="V86" s="15" t="s">
@@ -11219,24 +11277,24 @@
       </c>
       <c r="N87" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O87" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P87" s="3" t="s">
         <v>390</v>
       </c>
       <c r="Q87" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R87" s="13"/>
       <c r="S87" s="11"/>
       <c r="T87" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Odessa&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/05/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Odessa&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U87" s="15"/>
       <c r="V87" s="15" t="s">
@@ -11285,11 +11343,11 @@
       </c>
       <c r="N88" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O88" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Doble Titulación</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>395</v>
@@ -11302,7 +11360,7 @@
       <c r="S88" s="11"/>
       <c r="T88" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Adrienne&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;05/03/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Adrienne&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U88" s="15"/>
       <c r="V88" s="15" t="s">
@@ -11355,20 +11413,20 @@
       </c>
       <c r="O89" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P89" s="3" t="s">
         <v>400</v>
       </c>
       <c r="Q89" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R89" s="13"/>
       <c r="S89" s="11"/>
       <c r="T89" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Charity&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;08/01/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Charity&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U89" s="15"/>
       <c r="V89" s="15" t="s">
@@ -11417,24 +11475,24 @@
       </c>
       <c r="N90" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O90" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P90" s="9" t="s">
         <v>405</v>
       </c>
       <c r="Q90" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R90" s="13"/>
       <c r="S90" s="11"/>
       <c r="T90" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Kieran&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Kieran&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U90" s="15"/>
       <c r="V90" s="15" t="s">
@@ -11483,24 +11541,24 @@
       </c>
       <c r="N91" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O91" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Semestre Académico</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P91" s="3" t="s">
         <v>411</v>
       </c>
       <c r="Q91" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R91" s="13"/>
       <c r="S91" s="11"/>
       <c r="T91" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Alika&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Alika&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U91" s="15"/>
       <c r="V91" s="15" t="s">
@@ -11549,24 +11607,24 @@
       </c>
       <c r="N92" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O92" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado Impacta Brasil</v>
+        <v>Prácticas</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>416</v>
       </c>
       <c r="Q92" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R92" s="13"/>
       <c r="S92" s="11"/>
       <c r="T92" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Shay&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Shay&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U92" s="15"/>
       <c r="V92" s="15" t="s">
@@ -11615,24 +11673,24 @@
       </c>
       <c r="N93" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O93" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado Impacta Brasil</v>
+        <v>Prácticas</v>
       </c>
       <c r="P93" s="3" t="s">
         <v>419</v>
       </c>
       <c r="Q93" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R93" s="13"/>
       <c r="S93" s="11"/>
       <c r="T93" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Cailin&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/02/2012&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Cailin&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U93" s="15"/>
       <c r="V93" s="15" t="s">
@@ -11681,24 +11739,24 @@
       </c>
       <c r="N94" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O94" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P94" s="5" t="s">
         <v>424</v>
       </c>
       <c r="Q94" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R94" s="13"/>
       <c r="S94" s="11"/>
       <c r="T94" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Xena&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval de Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Xena&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U94" s="15"/>
       <c r="V94" s="15" t="s">
@@ -11716,7 +11774,7 @@
       <c r="Z94" s="21"/>
       <c r="AA94" s="21"/>
     </row>
-    <row r="95" spans="2:27" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:27" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="3">
         <v>87</v>
       </c>
@@ -11751,20 +11809,20 @@
       </c>
       <c r="O95" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta Perú</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P95" s="3" t="s">
         <v>430</v>
       </c>
       <c r="Q95" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R95" s="13"/>
       <c r="S95" s="11"/>
       <c r="T95" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Walker&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Walker&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U95" s="15"/>
       <c r="V95" s="15" t="s">
@@ -11813,24 +11871,24 @@
       </c>
       <c r="N96" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O96" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Leadership And Global Understanding - Summer Program</v>
+        <v>Summer Programme Responsible Management Rennes</v>
       </c>
       <c r="P96" s="5" t="s">
         <v>434</v>
       </c>
       <c r="Q96" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
       </c>
       <c r="R96" s="13"/>
       <c r="S96" s="11"/>
       <c r="T96" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Adena&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Adena&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U96" s="15"/>
       <c r="V96" s="15" t="s">
@@ -11879,24 +11937,24 @@
       </c>
       <c r="N97" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O97" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Korean Studies Summer Program Hannam University</v>
+        <v>Summer Programme Responsible Management Rennes</v>
       </c>
       <c r="P97" s="3" t="s">
         <v>440</v>
       </c>
       <c r="Q97" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R97" s="13"/>
       <c r="S97" s="11"/>
       <c r="T97" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Bradley&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;11/05/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Bradley&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U97" s="15"/>
       <c r="V97" s="15" t="s">
@@ -11945,11 +12003,11 @@
       </c>
       <c r="N98" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2017</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O98" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Prácticas</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P98" s="5" t="s">
         <v>445</v>
@@ -11962,7 +12020,7 @@
       <c r="S98" s="11"/>
       <c r="T98" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Yvette&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/02/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Yvette&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U98" s="15"/>
       <c r="V98" s="15" t="s">
@@ -12011,24 +12069,24 @@
       </c>
       <c r="N99" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O99" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Gira Académica Italia</v>
+        <v>Voluntariado impacta México</v>
       </c>
       <c r="P99" s="3" t="s">
         <v>450</v>
       </c>
       <c r="Q99" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;</v>
       </c>
       <c r="R99" s="13"/>
       <c r="S99" s="11"/>
       <c r="T99" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;Neil&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Neil&lt;/td&gt;&lt;td class="text-success"&gt;Aprobado&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U99" s="15"/>
       <c r="V99" s="15" t="s">
@@ -12077,24 +12135,24 @@
       </c>
       <c r="N100" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRIMER SEMESTRE 2018</v>
+        <v>JUNIO A JULIO 2018</v>
       </c>
       <c r="O100" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta México</v>
+        <v>Leadership And Global Understanding - Summer Program</v>
       </c>
       <c r="P100" s="5" t="s">
         <v>455</v>
       </c>
       <c r="Q100" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
       </c>
       <c r="R100" s="13"/>
       <c r="S100" s="11"/>
       <c r="T100" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Hunter&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/01/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Leadership And Global Understanding - Summer Program&lt;/td&gt;&lt;td&gt;Hunter&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U100" s="15"/>
       <c r="V100" s="15" t="s">
@@ -12112,7 +12170,7 @@
       <c r="Z100" s="21"/>
       <c r="AA100" s="21"/>
     </row>
-    <row r="101" spans="2:27" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:27" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B101" s="3">
         <v>93</v>
       </c>
@@ -12143,24 +12201,24 @@
       </c>
       <c r="N101" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O101" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Semestre Académico</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P101" s="3" t="s">
         <v>460</v>
       </c>
       <c r="Q101" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R101" s="13"/>
       <c r="S101" s="11"/>
       <c r="T101" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Marcia&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/05/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Marcia&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U101" s="15"/>
       <c r="V101" s="15" t="s">
@@ -12209,24 +12267,24 @@
       </c>
       <c r="N102" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>SEGUNDO SEMESTRE 2018</v>
       </c>
       <c r="O102" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta México</v>
+        <v>Prácticas</v>
       </c>
       <c r="P102" s="5" t="s">
         <v>465</v>
       </c>
       <c r="Q102" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;</v>
       </c>
       <c r="R102" s="13"/>
       <c r="S102" s="11"/>
       <c r="T102" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Lavinia&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;01/12/2013&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Lavinia&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U102" s="15"/>
       <c r="V102" s="15" t="s">
@@ -12275,24 +12333,24 @@
       </c>
       <c r="N103" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>PRIMER SEMESTRE 2018</v>
       </c>
       <c r="O103" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Semestre Académico</v>
+        <v>Korean Studies Summer Program Hannam University</v>
       </c>
       <c r="P103" s="3" t="s">
         <v>469</v>
       </c>
       <c r="Q103" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R103" s="13"/>
       <c r="S103" s="11"/>
       <c r="T103" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;Cynthia&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;02/06/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2018&lt;/td&gt;&lt;td&gt;Korean Studies Summer Program Hannam University&lt;/td&gt;&lt;td&gt;Cynthia&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U103" s="15"/>
       <c r="V103" s="15" t="s">
@@ -12341,7 +12399,7 @@
       </c>
       <c r="N104" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O104" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -12358,7 +12416,7 @@
       <c r="S104" s="11"/>
       <c r="T104" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Lee&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;03/04/2014&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado impacta Perú&lt;/td&gt;&lt;td&gt;Lee&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U104" s="15"/>
       <c r="V104" s="15" t="s">
@@ -12407,24 +12465,24 @@
       </c>
       <c r="N105" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2018 A ENERO 2019</v>
       </c>
       <c r="O105" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Misión Técnica Ingeniería</v>
+        <v>Voluntariado Impacta Brasil</v>
       </c>
       <c r="P105" s="3" t="s">
         <v>480</v>
       </c>
       <c r="Q105" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;</v>
       </c>
       <c r="R105" s="13"/>
       <c r="S105" s="11"/>
       <c r="T105" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;Linda&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;12/12/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;Linda&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Coordinador Programa)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U105" s="15"/>
       <c r="V105" s="15" t="s">
@@ -12473,24 +12531,24 @@
       </c>
       <c r="N106" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O106" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Prácticas</v>
+        <v>Doble Titulación</v>
       </c>
       <c r="P106" s="5" t="s">
         <v>485</v>
       </c>
       <c r="Q106" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R106" s="13"/>
       <c r="S106" s="11"/>
       <c r="T106" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Prácticas&lt;/td&gt;&lt;td&gt;Wayne&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII 2ª Carga)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/11/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Doble Titulación&lt;/td&gt;&lt;td&gt;Wayne&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U106" s="15"/>
       <c r="V106" s="15" t="s">
@@ -12508,7 +12566,7 @@
       <c r="Z106" s="21"/>
       <c r="AA106" s="21"/>
     </row>
-    <row r="107" spans="2:27" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:27" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="3">
         <v>99</v>
       </c>
@@ -12539,24 +12597,24 @@
       </c>
       <c r="N107" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O107" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Voluntariado impacta México</v>
+        <v xml:space="preserve">  Gira Académica a Perú</v>
       </c>
       <c r="P107" s="3" t="s">
         <v>489</v>
       </c>
       <c r="Q107" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;</v>
       </c>
       <c r="R107" s="13"/>
       <c r="S107" s="11"/>
       <c r="T107" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Voluntariado impacta México&lt;/td&gt;&lt;td&gt;Liberty&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;06/09/2014&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;  Gira Académica a Perú&lt;/td&gt;&lt;td&gt;Liberty&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U107" s="15"/>
       <c r="V107" s="15" t="s">
@@ -12605,24 +12663,24 @@
       </c>
       <c r="N108" s="11" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DICIEMBRE 2018 A ENERO 2019</v>
+        <v>JUNIO A JULIO 2017</v>
       </c>
       <c r="O108" s="11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Summer Program Introduction to Materials Science and Enginnering</v>
       </c>
       <c r="P108" s="5" t="s">
         <v>495</v>
       </c>
       <c r="Q108" s="11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R108" s="13"/>
       <c r="S108" s="11"/>
       <c r="T108" s="15" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;DICIEMBRE 2018 A ENERO 2019&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;Cathleen&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;09/02/2013&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2017&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;Cathleen&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U108" s="15"/>
       <c r="V108" s="15" t="s">
@@ -12640,7 +12698,7 @@
       <c r="Z108" s="21"/>
       <c r="AA108" s="21"/>
     </row>
-    <row r="109" spans="2:27" ht="102" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:27" ht="127.5" x14ac:dyDescent="0.25">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -12654,22 +12712,22 @@
       <c r="M109" s="19"/>
       <c r="N109" s="11" t="str">
         <f t="shared" ref="N109:N113" ca="1" si="9">INDEX(I$9:I$16,RANDBETWEEN(1,COUNTA(I$9:I$16)))</f>
-        <v>SEGUNDO SEMESTRE 2017</v>
+        <v>DICIEMBRE 2017 A ENERO 2018</v>
       </c>
       <c r="O109" s="13" t="str">
         <f t="shared" ref="O109:O113" ca="1" si="10">INDEX(K$9:K$21,RANDBETWEEN(1,COUNTA(K$9:K$21)))</f>
-        <v>Gira Académica Italia</v>
+        <v>Misión Técnica Ingeniería</v>
       </c>
       <c r="P109" s="5"/>
       <c r="Q109" s="13" t="str">
         <f t="shared" ref="Q109:Q113" ca="1" si="11">INDEX(J$9:J$22,RANDBETWEEN(1,COUNTA(J$9:J$22)))</f>
-        <v>&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R109" s="20"/>
       <c r="S109" s="11"/>
       <c r="T109" s="21" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Cancelado&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Misión Técnica Ingeniería&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U109" s="21"/>
       <c r="V109" s="15" t="s">
@@ -12687,7 +12745,7 @@
       <c r="Z109" s="21"/>
       <c r="AA109" s="21"/>
     </row>
-    <row r="110" spans="2:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:27" ht="102" x14ac:dyDescent="0.25">
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -12701,7 +12759,7 @@
       <c r="M110" s="19"/>
       <c r="N110" s="11" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PRIMER SEMESTRE 2017</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O110" s="13" t="str">
         <f t="shared" ca="1" si="10"/>
@@ -12710,13 +12768,13 @@
       <c r="P110" s="11"/>
       <c r="Q110" s="13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R110" s="13"/>
       <c r="S110" s="11"/>
       <c r="T110" s="21" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U110" s="21"/>
       <c r="V110" s="15"/>
@@ -12726,7 +12784,7 @@
       <c r="Z110" s="21"/>
       <c r="AA110" s="21"/>
     </row>
-    <row r="111" spans="2:27" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:27" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
@@ -12740,22 +12798,22 @@
       <c r="M111" s="19"/>
       <c r="N111" s="11" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DICIEMBRE 2017 A ENERO 2018</v>
+        <v>PRIMER SEMESTRE 2017</v>
       </c>
       <c r="O111" s="13" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Summer Program Introduction to Materials Science and Enginnering</v>
+        <v>Semestre Académico</v>
       </c>
       <c r="P111" s="11"/>
       <c r="Q111" s="13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
       </c>
       <c r="R111" s="13"/>
       <c r="S111" s="11"/>
       <c r="T111" s="21" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;DICIEMBRE 2017 A ENERO 2018&lt;/td&gt;&lt;td&gt;Summer Program Introduction to Materials Science and Enginnering&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-info"&gt;En Trámite (Esperando Aval Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;PRIMER SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U111" s="21"/>
       <c r="V111" s="15"/>
@@ -12765,7 +12823,7 @@
       <c r="Z111" s="21"/>
       <c r="AA111" s="21"/>
     </row>
-    <row r="112" spans="2:27" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:27" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
@@ -12779,22 +12837,22 @@
       <c r="M112" s="19"/>
       <c r="N112" s="11" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O112" s="13" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Semestre Académico</v>
+        <v>Gira Académica Italia</v>
       </c>
       <c r="P112" s="11"/>
       <c r="Q112" s="13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;</v>
       </c>
       <c r="R112" s="13"/>
       <c r="S112" s="11"/>
       <c r="T112" s="21" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Semestre Académico&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Gira Académica Italia&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Vicerrectoría)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U112" s="21"/>
       <c r="V112" s="15" t="s">
@@ -12812,7 +12870,7 @@
       <c r="Z112" s="21"/>
       <c r="AA112" s="21"/>
     </row>
-    <row r="113" spans="2:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:27" ht="102" x14ac:dyDescent="0.25">
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
@@ -12826,22 +12884,22 @@
       <c r="M113" s="19"/>
       <c r="N113" s="11" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JUNIO A JULIO 2018</v>
+        <v>SEGUNDO SEMESTRE 2017</v>
       </c>
       <c r="O113" s="13" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Summer Programme Responsible Management Rennes</v>
+        <v>Voluntariado Impacta Brasil</v>
       </c>
       <c r="P113" s="11"/>
       <c r="Q113" s="13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;</v>
+        <v>&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;</v>
       </c>
       <c r="R113" s="13"/>
       <c r="S113" s="11"/>
       <c r="T113" s="21" t="str">
         <f ca="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",TEXT(Tabla1[[#This Row],[Fecha de Pre-Registro]], "dd/mm/aaaa"),"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[PERIODO]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Modalidad]],"&lt;/td&gt;&lt;td&gt;",Tabla1[[#This Row],[Nombres]],"&lt;/td&gt;",Tabla1[[#This Row],[Estado]],"",IF(Tabla1[[#This Row],[Estado]]=J$10,"&lt;td&gt;&lt;/td&gt;","&lt;td&gt;&lt;a class=""btn btn-danger"" href=""javascript:void(0);"" title=""Cancelar movilidad del estudiante""&gt;&lt;i class=""fa fa-remove""&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;"),"&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;JUNIO A JULIO 2018&lt;/td&gt;&lt;td&gt;Summer Programme Responsible Management Rennes&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (ORII)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;00/01/1900&lt;/td&gt;&lt;td&gt;SEGUNDO SEMESTRE 2017&lt;/td&gt;&lt;td&gt;Voluntariado Impacta Brasil&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td class="text-danger"&gt;Rechazado (Institución de Destino)&lt;/td&gt;&lt;td&gt;&lt;a class="btn btn-danger" href="javascript:void(0);" title="Cancelar movilidad del estudiante"&gt;&lt;i class="fa fa-remove"&gt;&lt;/i&gt; Cancelar&lt;/a&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="U113" s="21"/>
       <c r="V113" s="15" t="s">
@@ -12875,7 +12933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z418"/>
   <sheetViews>
-    <sheetView topLeftCell="F61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -17251,8 +17309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22390,4 +22448,543 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37">
+        <v>1</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>2</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="37">
+        <v>3</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="37">
+        <v>4</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="37">
+        <v>6</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="37">
+        <v>7</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="37">
+        <v>8</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f>LOOKUP(C10,$A$1:$B$8,$B$1:$B$8)</f>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E10" t="str">
+        <f>CONCATENATE("('",A10," ",,B10,"',",C10,"),")</f>
+        <v>('EMAIL - REGISTRO DATOS EL USUARIO',1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" ref="D11:D33" si="0">LOOKUP(C11,$A$1:$B$8,$B$1:$B$8)</f>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" ref="E11:E33" si="1">CONCATENATE("('",A11," ",,B11,"',",C11,"),")</f>
+        <v>('EMAIL - RECHAZADO POR EL VALIDADOR',1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - APROBADO POR EL VALIDADOR',1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA POR EL VALIDADOR',1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - VENCIDA PARA INVOLUCRADOS',1),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>INICIATIVA</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA PARA INVOLUCRADOS',1),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - REGISTRO DATOS EL USUARIO',2),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - RECHAZADO POR EL VALIDADOR',2),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - APROBADO POR EL VALIDADOR',2),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA POR EL VALIDADOR',2),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - VENCIDA PARA INVOLUCRADOS',2),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSCRIPCION</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA PARA INVOLUCRADOS',2),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>OPORTUNIDAD</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - REGISTRO DATOS EL USUARIO',4),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>OPORTUNIDAD</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - VENCIDA PARA INVOLUCRADOS',4),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>OPORTUNIDAD</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA PARA INVOLUCRADOS',4),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - REGISTRO DATOS EL USUARIO',6),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - REGISTRO DATOS EL USUARIO EXTERNO',6),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACEPTADO POR EL USUARIO EXTERNO',6),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - DECLINADO POR EL USUARIO EXTERNO',6),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - RECHAZADO POR EL VALIDADOR',6),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - APROBADO POR EL VALIDADOR',6),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA POR EL VALIDADOR',6),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - VENCIDA PARA INVOLUCRADOS',6),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>ALIANZA</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>('EMAIL - ACTIVA PARA INVOLUCRADOS',6),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>